<commit_message>
update new vacc rki
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2021-04-18.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2021-04-18.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="303">
   <si>
     <t xml:space="preserve">Testungen</t>
   </si>
@@ -747,22 +747,22 @@
     <t xml:space="preserve">Geimpfte Personen</t>
   </si>
   <si>
-    <t xml:space="preserve">Stand 20.4.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16795784 (20,2 %)</t>
+    <t xml:space="preserve">Stand 21.4.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17288804 (20,8 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Mit nur 1 Impfung</t>
   </si>
   <si>
-    <t xml:space="preserve">11212792 (13,5 %)</t>
+    <t xml:space="preserve">11642016 (14,0 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Mit 2 Impfungen</t>
   </si>
   <si>
-    <t xml:space="preserve">5582992 ( 6,7 %)</t>
+    <t xml:space="preserve">5646788 ( 6,8 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Impffortschritt</t>
@@ -810,85 +810,76 @@
     <t xml:space="preserve">Gesamt 2x</t>
   </si>
   <si>
+    <t xml:space="preserve">20,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21,4</t>
+  </si>
+  <si>
     <t xml:space="preserve">20,2</t>
   </si>
   <si>
-    <t xml:space="preserve">6,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19,3</t>
+    <t xml:space="preserve">8,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21,6</t>
   </si>
   <si>
     <t xml:space="preserve">6,6</t>
   </si>
   <si>
-    <t xml:space="preserve">20,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,2</t>
+    <t xml:space="preserve">23,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,7</t>
   </si>
   <si>
     <t xml:space="preserve">20,4</t>
   </si>
   <si>
-    <t xml:space="preserve">5,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20,5</t>
+    <t xml:space="preserve">21,3</t>
   </si>
   <si>
     <t xml:space="preserve">6,2</t>
   </si>
   <si>
-    <t xml:space="preserve">22,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,2</t>
+    <t xml:space="preserve">20,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,3</t>
   </si>
   <si>
     <t xml:space="preserve">Impfstoffdosen</t>
@@ -900,19 +891,19 @@
     <t xml:space="preserve">Biontech/Pfizer</t>
   </si>
   <si>
-    <t xml:space="preserve">16526626 ( 93,8 %)</t>
+    <t xml:space="preserve">16905070 ( 96,0 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Erstimpfungen</t>
   </si>
   <si>
-    <t xml:space="preserve">11248051</t>
+    <t xml:space="preserve">11571347</t>
   </si>
   <si>
     <t xml:space="preserve">Zweitimpfungen</t>
   </si>
   <si>
-    <t xml:space="preserve">5278575</t>
+    <t xml:space="preserve">5333723</t>
   </si>
   <si>
     <t xml:space="preserve">geliefert</t>
@@ -924,13 +915,13 @@
     <t xml:space="preserve">Moderna</t>
   </si>
   <si>
-    <t xml:space="preserve">1204361 (  6,8 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">908286</t>
-  </si>
-  <si>
-    <t xml:space="preserve">296075</t>
+    <t xml:space="preserve">1242388 (  7,1 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">939534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">302854</t>
   </si>
   <si>
     <t xml:space="preserve">1759562</t>
@@ -939,13 +930,13 @@
     <t xml:space="preserve">AstraZeneca</t>
   </si>
   <si>
-    <t xml:space="preserve">4647789 ( 26,4 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4639447</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8342</t>
+    <t xml:space="preserve">4788134 ( 27,2 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4777923</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10211</t>
   </si>
   <si>
     <t xml:space="preserve">5937600</t>
@@ -1518,7 +1509,7 @@
         <v>263</v>
       </c>
       <c r="D4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E4" t="n">
         <v>186</v>
@@ -1535,10 +1526,10 @@
         <v>43346</v>
       </c>
       <c r="C5" t="s">
+        <v>264</v>
+      </c>
+      <c r="D5" t="s">
         <v>265</v>
-      </c>
-      <c r="D5" t="s">
-        <v>266</v>
       </c>
       <c r="E5" t="n">
         <v>140</v>
@@ -1555,7 +1546,7 @@
         <v>40481</v>
       </c>
       <c r="C6" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D6" t="s">
         <v>262</v>
@@ -1575,10 +1566,10 @@
         <v>7986</v>
       </c>
       <c r="C7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E7" t="n">
         <v>169</v>
@@ -1595,10 +1586,10 @@
         <v>21712</v>
       </c>
       <c r="C8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E8" t="n">
         <v>131</v>
@@ -1615,10 +1606,10 @@
         <v>69185</v>
       </c>
       <c r="C9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D9" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E9" t="n">
         <v>156</v>
@@ -1635,10 +1626,10 @@
         <v>37741</v>
       </c>
       <c r="C10" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="D10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E10" t="n">
         <v>138</v>
@@ -1655,10 +1646,10 @@
         <v>103794</v>
       </c>
       <c r="C11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E11" t="n">
         <v>121</v>
@@ -1675,10 +1666,10 @@
         <v>283887</v>
       </c>
       <c r="C12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D12" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="E12" t="n">
         <v>171</v>
@@ -1695,10 +1686,10 @@
         <v>54705</v>
       </c>
       <c r="C13" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="D13" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="E13" t="n">
         <v>139</v>
@@ -1715,10 +1706,10 @@
         <v>13743</v>
       </c>
       <c r="C14" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D14" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E14" t="n">
         <v>128</v>
@@ -1735,10 +1726,10 @@
         <v>60658</v>
       </c>
       <c r="C15" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D15" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="E15" t="n">
         <v>206</v>
@@ -1755,10 +1746,10 @@
         <v>30302</v>
       </c>
       <c r="C16" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="D16" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E16" t="n">
         <v>175</v>
@@ -1775,10 +1766,10 @@
         <v>37438</v>
       </c>
       <c r="C17" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D17" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E17" t="n">
         <v>72</v>
@@ -1795,10 +1786,10 @@
         <v>26037</v>
       </c>
       <c r="C18" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="D18" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E18" t="n">
         <v>241</v>
@@ -1823,106 +1814,106 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B6" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B7" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B8" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B9" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B10" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B11" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B12" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B13" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>